<commit_message>
- Add fabrics table to data base - Refactor the get_data function to make the data suitable to recreated database - Recreat db_save_main_info function
</commit_message>
<xml_diff>
--- a/Apparel Merchandisers Helper/DB/DB Management.xlsx
+++ b/Apparel Merchandisers Helper/DB/DB Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyData\learn\WebDevolopment\WorkSpace\Apparel-Merchandisers-Helper\Apparel Merchandisers Helper\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyData\learn\Programming\WorkSpace\Apparel-Merchandisers-Helper\Apparel Merchandisers Helper\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAB6BF5-F288-4635-B2A2-E02DA11422B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B1EB72-6BF4-4ABA-B551-C1D9EDCF559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Primary key</t>
   </si>
   <si>
-    <t>Paking Method</t>
-  </si>
-  <si>
     <t>Total QTY</t>
   </si>
   <si>
@@ -75,15 +72,9 @@
     <t>style_name</t>
   </si>
   <si>
-    <t>team/color</t>
-  </si>
-  <si>
     <t>team</t>
   </si>
   <si>
-    <t>color_combo</t>
-  </si>
-  <si>
     <t>piece1 color</t>
   </si>
   <si>
@@ -115,6 +106,15 @@
   </si>
   <si>
     <t>color_qty</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>color_code</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="B1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,12 +518,12 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="J2" s="8" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>4</v>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="L3" s="3"/>
     </row>
@@ -570,13 +570,13 @@
         <v>3</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="5">
         <v>2</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -592,14 +592,14 @@
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="3"/>
       <c r="J5" s="5">
         <v>3</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L5" s="3"/>
     </row>
@@ -608,24 +608,24 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3"/>
       <c r="F6" s="4">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="3"/>
       <c r="J6" s="5">
         <v>4</v>
       </c>
       <c r="K6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -633,21 +633,21 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3"/>
       <c r="F7" s="4">
         <v>5</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="3"/>
       <c r="J7" s="5">
         <v>5</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L7" s="3"/>
     </row>
@@ -656,23 +656,23 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="F8" s="4">
         <v>6</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H8" s="3"/>
       <c r="J8" s="5">
         <v>6</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L8" s="3"/>
     </row>
@@ -681,14 +681,14 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3"/>
       <c r="F9" s="4">
         <v>7</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H9" s="3"/>
       <c r="J9" s="5">
@@ -702,7 +702,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="4">
@@ -721,7 +721,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3"/>
       <c r="F11" s="4">
@@ -740,7 +740,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3"/>
       <c r="F12" s="4">
@@ -759,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3"/>
       <c r="F13" s="4">
@@ -778,7 +778,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3"/>
       <c r="F14" s="4">
@@ -797,7 +797,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D15" s="3"/>
       <c r="F15" s="4">

</xml_diff>